<commit_message>
Updated docs, removed extra column
</commit_message>
<xml_diff>
--- a/src/nbin_golf/TestOrders.xlsx
+++ b/src/nbin_golf/TestOrders.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dougransom.sharepoint.com/sites/operations2/Shared Documents/scripts/bulk mutual funds/src/nbin_golf/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A0E1837-4E1C-405D-BCBE-F8509C7203D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{2A0E1837-4E1C-405D-BCBE-F8509C7203D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C3941B2-1935-4D19-ACCA-8A81D5000F65}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="3540" windowWidth="17280" windowHeight="9420"/>
+    <workbookView xWindow="7140" yWindow="3825" windowWidth="21600" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestOrders" sheetId="1" r:id="rId1"/>
@@ -151,18 +151,12 @@
     <t>fund5</t>
   </si>
   <si>
-    <t>ABCD4193</t>
-  </si>
-  <si>
     <t>93361Z</t>
   </si>
   <si>
     <t>fund6</t>
   </si>
   <si>
-    <t>ABCD4194</t>
-  </si>
-  <si>
     <t>92145H</t>
   </si>
   <si>
@@ -172,28 +166,34 @@
     <t>fund7</t>
   </si>
   <si>
-    <t>ABCD4195</t>
-  </si>
-  <si>
     <t>94434J</t>
   </si>
   <si>
     <t>fund8</t>
   </si>
   <si>
-    <t>ABCD4196</t>
-  </si>
-  <si>
     <t>92737M</t>
   </si>
   <si>
     <t>Sell All</t>
+  </si>
+  <si>
+    <t>abc3903</t>
+  </si>
+  <si>
+    <t>def39093</t>
+  </si>
+  <si>
+    <t>def390347</t>
+  </si>
+  <si>
+    <t>def30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1028,16 +1028,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="25.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -1096,7 +1100,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1153,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1321,7 +1325,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1362,10 +1366,10 @@
         <v>42</v>
       </c>
       <c r="O6" t="s">
+        <v>52</v>
+      </c>
+      <c r="P6" t="s">
         <v>43</v>
-      </c>
-      <c r="P6" t="s">
-        <v>44</v>
       </c>
       <c r="Q6" t="s">
         <v>21</v>
@@ -1377,7 +1381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1418,13 +1422,13 @@
         <v>24</v>
       </c>
       <c r="N7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" t="s">
         <v>45</v>
-      </c>
-      <c r="O7" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" t="s">
-        <v>47</v>
       </c>
       <c r="Q7" t="s">
         <v>21</v>
@@ -1433,10 +1437,10 @@
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1474,13 +1478,13 @@
         <v>24</v>
       </c>
       <c r="N8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="P8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q8" t="s">
         <v>21</v>
@@ -1492,7 +1496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1531,13 +1535,13 @@
         <v>24</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="O9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="Q9" t="s">
         <v>21</v>
@@ -1805,13 +1809,45 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A900687A-FF40-470A-BE58-609F33D5E16C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A900687A-FF40-470A-BE58-609F33D5E16C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f01d5297-5609-48f6-bc3b-4288ccc4bf80"/>
+    <ds:schemaRef ds:uri="c4a35957-e4dc-4fc1-815b-5c596c4ca67d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63DE3E0-118E-4696-B29E-320EF58B1962}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D63DE3E0-118E-4696-B29E-320EF58B1962}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4FA3FE1-51C0-43E4-96EE-569A356CA2FE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4FA3FE1-51C0-43E4-96EE-569A356CA2FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4a35957-e4dc-4fc1-815b-5c596c4ca67d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="f01d5297-5609-48f6-bc3b-4288ccc4bf80"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>